<commit_message>
updated rotor weight trend data
</commit_message>
<xml_diff>
--- a/docs/rotors/rotor_data.xlsx
+++ b/docs/rotors/rotor_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alfiyandyhr/Github_Repos/MCEVS/docs/rotors/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57AE71DC-9AE8-934B-8D3D-367EF7276B79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2127878B-A188-0146-848D-F7D5EDE7BC04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17180" xr2:uid="{2F87124F-FADD-1C4B-8E1F-F5E2F237BAFB}"/>
   </bookViews>
@@ -2093,8 +2093,8 @@
       <cdr:x>0.83884</cdr:x>
       <cdr:y>0.81918</cdr:y>
     </cdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <cdr:sp macro="" textlink="">
           <cdr:nvSpPr>
             <cdr:cNvPr id="2" name="TextBox 36">
@@ -2349,7 +2349,7 @@
           </cdr:txBody>
         </cdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <cdr:sp macro="" textlink="">
           <cdr:nvSpPr>
             <cdr:cNvPr id="2" name="TextBox 36">
@@ -2537,8 +2537,8 @@
       <cdr:x>0.49151</cdr:x>
       <cdr:y>0.39962</cdr:y>
     </cdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <cdr:sp macro="" textlink="">
           <cdr:nvSpPr>
             <cdr:cNvPr id="3" name="TextBox 36">
@@ -2796,7 +2796,7 @@
           </cdr:txBody>
         </cdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <cdr:sp macro="" textlink="">
           <cdr:nvSpPr>
             <cdr:cNvPr id="3" name="TextBox 36">
@@ -2987,8 +2987,8 @@
       <cdr:x>0.62599</cdr:x>
       <cdr:y>0.20843</cdr:y>
     </cdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <cdr:sp macro="" textlink="">
           <cdr:nvSpPr>
             <cdr:cNvPr id="4" name="TextBox 36">
@@ -3227,7 +3227,7 @@
           </cdr:txBody>
         </cdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <cdr:sp macro="" textlink="">
           <cdr:nvSpPr>
             <cdr:cNvPr id="4" name="TextBox 36">
@@ -3418,8 +3418,8 @@
       <cdr:x>0.48772</cdr:x>
       <cdr:y>0.56957</cdr:y>
     </cdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <cdr:sp macro="" textlink="">
           <cdr:nvSpPr>
             <cdr:cNvPr id="5" name="TextBox 36">
@@ -3676,7 +3676,7 @@
           </cdr:txBody>
         </cdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <cdr:sp macro="" textlink="">
           <cdr:nvSpPr>
             <cdr:cNvPr id="5" name="TextBox 36">
@@ -4174,7 +4174,7 @@
   <dimension ref="B2:K41"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="F34" sqref="F34"/>
+      <selection activeCell="H41" sqref="H41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
updated rotor weight data
</commit_message>
<xml_diff>
--- a/docs/rotors/rotor_data.xlsx
+++ b/docs/rotors/rotor_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alfiyandyhr/Github_Repos/MCEVS/docs/rotors/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2127878B-A188-0146-848D-F7D5EDE7BC04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16AD7EF9-59F9-2D4C-B8C9-CD0CC7996953}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17180" xr2:uid="{2F87124F-FADD-1C4B-8E1F-F5E2F237BAFB}"/>
   </bookViews>
@@ -4173,8 +4173,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83E76DEE-66FE-6E46-8276-3145E42439BE}">
   <dimension ref="B2:K41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="H41" sqref="H41"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>